<commit_message>
Washington Huskies Uniform Updates
</commit_message>
<xml_diff>
--- a/textures/SLUS-21214/replacements/uniforms/FBS/Washington/Washington.xlsx
+++ b/textures/SLUS-21214/replacements/uniforms/FBS/Washington/Washington.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PCSX2\textures\SLUS-21214\replacements\uniforms\FBS\Washington\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100A2E62-65C4-43DF-8222-C612A42AA9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DD1980-1DA8-493E-B211-2D0B87EAF977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="4050" windowWidth="38700" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="38700" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UNIF" sheetId="2" r:id="rId1"/>
@@ -2963,60 +2963,6 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -3198,6 +3144,25 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3245,6 +3210,41 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3323,13 +3323,13 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="KIT" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{2F9953C0-79AB-4287-90F8-CA4305E2AA49}" name="Column1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="JERSEY" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PANTS" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="HELMET" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{21D90594-1113-4121-B9B7-1060F4A6FE2C}" name="Primary Glove" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{137CBB6B-E9F4-41A1-9A8E-0DEBDA14E5D4}" name="STATUS" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{2F9953C0-79AB-4287-90F8-CA4305E2AA49}" name="Column1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="JERSEY" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PANTS" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="HELMET" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{21D90594-1113-4121-B9B7-1060F4A6FE2C}" name="Primary Glove" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{137CBB6B-E9F4-41A1-9A8E-0DEBDA14E5D4}" name="STATUS" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3411,15 +3411,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C34D1828-392F-4E13-BA1B-A24EBF7BD5E7}" name="Table315" displayName="Table315" ref="K2:P22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C34D1828-392F-4E13-BA1B-A24EBF7BD5E7}" name="Table315" displayName="Table315" ref="K2:P22" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="K2:P22" xr:uid="{C34D1828-392F-4E13-BA1B-A24EBF7BD5E7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{23423812-DBD7-4F54-A81D-2D8AB4BDC06E}" name="KIT" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{6019954C-8FE0-4DCB-8D97-675F82CCB0B8}" name="JERSEY" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{E7859F15-258E-45FF-AAD5-F44C5A57D50C}" name="PANTS" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A9A89A21-322C-4074-BF9E-08373FE0C6FD}" name="HELMET" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{892C7663-AF95-46A0-9DBC-6F79D5485B94}" name="Name" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E6A207C7-A206-41AA-814F-B3633F9D823F}" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{23423812-DBD7-4F54-A81D-2D8AB4BDC06E}" name="KIT" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{6019954C-8FE0-4DCB-8D97-675F82CCB0B8}" name="JERSEY" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E7859F15-258E-45FF-AAD5-F44C5A57D50C}" name="PANTS" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A9A89A21-322C-4074-BF9E-08373FE0C6FD}" name="HELMET" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{892C7663-AF95-46A0-9DBC-6F79D5485B94}" name="Name" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E6A207C7-A206-41AA-814F-B3633F9D823F}" name="STATUS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3830,7 +3830,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A15" sqref="A15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>